<commit_message>
new list with Florida companies
</commit_message>
<xml_diff>
--- a/examples/TopSciTech.xlsx
+++ b/examples/TopSciTech.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10307"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jesusdelvalle/Documents/projects/make_slides/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jesusdelvalle/Documents/projects/make_slides/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5F3E9B4-3EA7-674C-8366-0059166EB158}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5B44CB7-78ED-6F42-BCBA-6ED1AEFFEFA9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="660" yWindow="640" windowWidth="21820" windowHeight="14040" xr2:uid="{7F6AFA6B-CF1A-42F3-8D13-BA0B0828C5F7}"/>
+    <workbookView xWindow="1840" yWindow="1020" windowWidth="25420" windowHeight="14040" xr2:uid="{7F6AFA6B-CF1A-42F3-8D13-BA0B0828C5F7}"/>
   </bookViews>
   <sheets>
     <sheet name="Companies" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="194">
   <si>
     <t>https://www.orchard-tx.com/</t>
   </si>
@@ -387,6 +387,234 @@
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Phoenix Tower International</t>
+  </si>
+  <si>
+    <t>Fanatiz</t>
+  </si>
+  <si>
+    <t>Neocis</t>
+  </si>
+  <si>
+    <t>Freightos</t>
+  </si>
+  <si>
+    <t>Metrc</t>
+  </si>
+  <si>
+    <t>Unybrands</t>
+  </si>
+  <si>
+    <t>Mayo Clinic</t>
+  </si>
+  <si>
+    <t>Longeveron</t>
+  </si>
+  <si>
+    <t>University of Florida</t>
+  </si>
+  <si>
+    <t>Oncology Analytics</t>
+  </si>
+  <si>
+    <t>Papa</t>
+  </si>
+  <si>
+    <t>ShipMonk</t>
+  </si>
+  <si>
+    <t>springbig</t>
+  </si>
+  <si>
+    <t>Jushi Holdings</t>
+  </si>
+  <si>
+    <t>Honorlock</t>
+  </si>
+  <si>
+    <t>InformedDNA</t>
+  </si>
+  <si>
+    <t>https://phoenixintnl.com/</t>
+  </si>
+  <si>
+    <t>https://www.fanatiz.com/</t>
+  </si>
+  <si>
+    <t>https://www.neocis.com/</t>
+  </si>
+  <si>
+    <t>https://www.freightos.com/</t>
+  </si>
+  <si>
+    <t>https://www.metrc.com/</t>
+  </si>
+  <si>
+    <t>https://unybrands.com/</t>
+  </si>
+  <si>
+    <t>https://www.mayoclinic.org/patient-visitor-guide/florida</t>
+  </si>
+  <si>
+    <t>https://www.longeveron.com/</t>
+  </si>
+  <si>
+    <t>https://www.ufl.edu/research/</t>
+  </si>
+  <si>
+    <t>https://www.oncologyanalytics.com/</t>
+  </si>
+  <si>
+    <t>https://honorlock.com/</t>
+  </si>
+  <si>
+    <t>https://informeddna.com/</t>
+  </si>
+  <si>
+    <t>Boca Raton, FL</t>
+  </si>
+  <si>
+    <t>Miami, FL</t>
+  </si>
+  <si>
+    <t>Miami, FL (Hong Kong)</t>
+  </si>
+  <si>
+    <t>Lakeland, FL</t>
+  </si>
+  <si>
+    <t>Jacksonville, FL</t>
+  </si>
+  <si>
+    <t>Gainesville, FL</t>
+  </si>
+  <si>
+    <t>St. Petersburg, FL</t>
+  </si>
+  <si>
+    <t>USA</t>
+  </si>
+  <si>
+    <t>Sports streaming platform.</t>
+  </si>
+  <si>
+    <t>Robotics technology for healthcare.</t>
+  </si>
+  <si>
+    <t>Online freight marketplace.</t>
+  </si>
+  <si>
+    <t>Top Medical Center, Hospital, Innovation Hub.</t>
+  </si>
+  <si>
+    <t>Cell Therapies for Aging-Related Chronic Diseases &amp; Conditions.</t>
+  </si>
+  <si>
+    <t>Innovation Academy, Innovation iHub, Inovation Square.</t>
+  </si>
+  <si>
+    <t>On-demand online exam proctoring services for schools and universities.</t>
+  </si>
+  <si>
+    <t>Counseling and Advising for health plans, health systems, and physicians, on the appropriate use of genetic testing.</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Telecommunication</t>
+  </si>
+  <si>
+    <t>Organs-on-chips to study toxicology and pharmacology of candidate medicines, chemicals, food.</t>
+  </si>
+  <si>
+    <t>https://hesperosinc.com/</t>
+  </si>
+  <si>
+    <t>Hesperos</t>
+  </si>
+  <si>
+    <t>Orlando, FL</t>
+  </si>
+  <si>
+    <t>Plantation, FL</t>
+  </si>
+  <si>
+    <t>https://www.joinpapa.com/</t>
+  </si>
+  <si>
+    <t>Mobile platform connecting care givers with seniors. Family-on-demand. Elder Tech. Aging.</t>
+  </si>
+  <si>
+    <t>https://www.shipmonk.com/</t>
+  </si>
+  <si>
+    <t>Order fulfillment for eCommerce. Supply chain management, inventory tracking. Logistics.</t>
+  </si>
+  <si>
+    <t>Fort Lauderdale, FL</t>
+  </si>
+  <si>
+    <t>Cannabis marketing platform.</t>
+  </si>
+  <si>
+    <t>https://springbig.com/</t>
+  </si>
+  <si>
+    <t>National, multi-state cannabis company developing and operating high-end retail locations, premium brands and state-of-the-art cultivation, processing and manufacturing facilities for Cannabis.</t>
+  </si>
+  <si>
+    <t>https://jushico.com/</t>
+  </si>
+  <si>
+    <t>Roper Technologies</t>
+  </si>
+  <si>
+    <t>Sarasota, FL</t>
+  </si>
+  <si>
+    <t>https://www.ropertech.com/</t>
+  </si>
+  <si>
+    <t>Diversified technology company of leading niche businesses that provide high gross-margins engineered products, software, and services.</t>
+  </si>
+  <si>
+    <t>Wireless infrastructure sites in global markets experiencing strong wireless usage growth.</t>
+  </si>
+  <si>
+    <t>Provider of regulatory, supply chain, track-and-trace solutions for the cannabis industry in the U.S.</t>
+  </si>
+  <si>
+    <t>eCommerce Platform. Acquires &amp; Maximizes Growth Potential for Online Brands. Targets successful Fulfillment by Amazon (FBA) and DTC sellers looking to scale their e-commerce businesses.</t>
+  </si>
+  <si>
+    <t>Provides health plans, providers, and patients with a data-driven, utilization management solution that delivers real-world, evidence-based analytics for Oncology.</t>
+  </si>
+  <si>
+    <t>Google</t>
+  </si>
+  <si>
+    <t>In Miami Google has Jobs involving their Google Cloud Solutions, Design, Financial Services...</t>
+  </si>
+  <si>
+    <t>Amazon</t>
+  </si>
+  <si>
+    <t>FL</t>
+  </si>
+  <si>
+    <t>All over the state, Jobs as Solutions Architect, Cloud Infrastructure Services, ...</t>
+  </si>
+  <si>
+    <t>https://careers.google.com/students/</t>
+  </si>
+  <si>
+    <t>https://www.amazon.jobs/en/business_categories/student-programs</t>
   </si>
 </sst>
 </file>
@@ -769,25 +997,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{287E21FB-93DB-4F7C-A8E2-BF4220365053}">
-  <dimension ref="A1:J31"/>
+  <dimension ref="A1:K51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.1640625" customWidth="1"/>
-    <col min="3" max="3" width="21.5" customWidth="1"/>
+    <col min="2" max="2" width="21.1640625" customWidth="1"/>
+    <col min="3" max="3" width="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" customWidth="1"/>
     <col min="6" max="6" width="7.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>82</v>
       </c>
@@ -810,16 +1040,19 @@
         <v>87</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -827,7 +1060,7 @@
         <v>76</v>
       </c>
       <c r="C2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>41</v>
@@ -841,14 +1074,17 @@
       <c r="G2">
         <v>2014</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2">
+        <v>2021</v>
+      </c>
+      <c r="I2" t="s">
         <v>48</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -856,7 +1092,7 @@
         <v>64</v>
       </c>
       <c r="C3" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>31</v>
@@ -870,14 +1106,17 @@
       <c r="G3">
         <v>2010</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3">
+        <v>2021</v>
+      </c>
+      <c r="I3" t="s">
         <v>6</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -885,7 +1124,7 @@
         <v>59</v>
       </c>
       <c r="C4" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>29</v>
@@ -899,17 +1138,20 @@
       <c r="G4">
         <v>2012</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4">
+        <v>2021</v>
+      </c>
+      <c r="I4" t="s">
         <v>6</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>2</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -917,7 +1159,7 @@
         <v>81</v>
       </c>
       <c r="C5" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>4</v>
@@ -931,17 +1173,20 @@
       <c r="G5">
         <v>2016</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5">
+        <v>2021</v>
+      </c>
+      <c r="I5" t="s">
         <v>5</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>6</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -949,7 +1194,7 @@
         <v>58</v>
       </c>
       <c r="C6" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>26</v>
@@ -963,14 +1208,17 @@
       <c r="G6">
         <v>2019</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6">
+        <v>2021</v>
+      </c>
+      <c r="I6" t="s">
         <v>28</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
@@ -978,7 +1226,7 @@
         <v>53</v>
       </c>
       <c r="C7" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -992,17 +1240,20 @@
       <c r="G7">
         <v>2015</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7">
+        <v>2021</v>
+      </c>
+      <c r="I7" t="s">
         <v>17</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>10</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1</v>
       </c>
@@ -1010,7 +1261,7 @@
         <v>80</v>
       </c>
       <c r="C8" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>0</v>
@@ -1024,17 +1275,20 @@
       <c r="G8">
         <v>2015</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8">
+        <v>2021</v>
+      </c>
+      <c r="I8" t="s">
         <v>2</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>3</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1</v>
       </c>
@@ -1042,7 +1296,7 @@
         <v>68</v>
       </c>
       <c r="C9" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>35</v>
@@ -1056,14 +1310,17 @@
       <c r="G9">
         <v>2008</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9">
+        <v>2021</v>
+      </c>
+      <c r="I9" t="s">
         <v>45</v>
       </c>
-      <c r="J9" t="s">
+      <c r="K9" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1</v>
       </c>
@@ -1071,7 +1328,7 @@
         <v>51</v>
       </c>
       <c r="C10" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>52</v>
@@ -1082,17 +1339,20 @@
       <c r="F10" t="s">
         <v>1</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H10">
+        <v>2021</v>
+      </c>
+      <c r="I10" t="s">
         <v>3</v>
       </c>
-      <c r="I10" t="s">
+      <c r="J10" t="s">
         <v>2</v>
       </c>
-      <c r="J10" t="s">
+      <c r="K10" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>1</v>
       </c>
@@ -1100,7 +1360,7 @@
         <v>56</v>
       </c>
       <c r="C11" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>24</v>
@@ -1114,14 +1374,17 @@
       <c r="G11">
         <v>2013</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H11">
+        <v>2021</v>
+      </c>
+      <c r="I11" t="s">
         <v>25</v>
       </c>
-      <c r="J11" t="s">
+      <c r="K11" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2</v>
       </c>
@@ -1129,7 +1392,7 @@
         <v>69</v>
       </c>
       <c r="C12" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>36</v>
@@ -1143,14 +1406,17 @@
       <c r="G12">
         <v>1990</v>
       </c>
-      <c r="H12" t="s">
+      <c r="H12">
+        <v>2021</v>
+      </c>
+      <c r="I12" t="s">
         <v>5</v>
       </c>
-      <c r="J12" t="s">
+      <c r="K12" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2</v>
       </c>
@@ -1158,7 +1424,7 @@
         <v>65</v>
       </c>
       <c r="C13" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>32</v>
@@ -1172,14 +1438,17 @@
       <c r="G13">
         <v>2013</v>
       </c>
-      <c r="H13" t="s">
+      <c r="H13">
+        <v>2021</v>
+      </c>
+      <c r="I13" t="s">
         <v>3</v>
       </c>
-      <c r="J13" t="s">
+      <c r="K13" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2</v>
       </c>
@@ -1187,7 +1456,7 @@
         <v>61</v>
       </c>
       <c r="C14" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>60</v>
@@ -1201,14 +1470,17 @@
       <c r="G14">
         <v>2013</v>
       </c>
-      <c r="H14" t="s">
+      <c r="H14">
+        <v>2021</v>
+      </c>
+      <c r="I14" t="s">
         <v>2</v>
       </c>
-      <c r="J14" t="s">
+      <c r="K14" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2</v>
       </c>
@@ -1216,7 +1488,7 @@
         <v>98</v>
       </c>
       <c r="C15" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>97</v>
@@ -1230,14 +1502,17 @@
       <c r="G15">
         <v>2007</v>
       </c>
-      <c r="H15" t="s">
+      <c r="H15">
+        <v>2021</v>
+      </c>
+      <c r="I15" t="s">
         <v>2</v>
       </c>
-      <c r="J15" t="s">
+      <c r="K15" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2</v>
       </c>
@@ -1245,7 +1520,7 @@
         <v>66</v>
       </c>
       <c r="C16" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>33</v>
@@ -1259,14 +1534,17 @@
       <c r="G16">
         <v>2012</v>
       </c>
-      <c r="H16" t="s">
+      <c r="H16">
+        <v>2021</v>
+      </c>
+      <c r="I16" t="s">
         <v>44</v>
       </c>
-      <c r="J16" t="s">
+      <c r="K16" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2</v>
       </c>
@@ -1274,7 +1552,7 @@
         <v>77</v>
       </c>
       <c r="C17" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>42</v>
@@ -1288,17 +1566,20 @@
       <c r="G17">
         <v>2013</v>
       </c>
-      <c r="H17" t="s">
+      <c r="H17">
+        <v>2021</v>
+      </c>
+      <c r="I17" t="s">
         <v>3</v>
       </c>
-      <c r="I17" t="s">
+      <c r="J17" t="s">
         <v>50</v>
       </c>
-      <c r="J17" t="s">
+      <c r="K17" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>2</v>
       </c>
@@ -1306,7 +1587,7 @@
         <v>57</v>
       </c>
       <c r="C18" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>13</v>
@@ -1320,17 +1601,20 @@
       <c r="G18">
         <v>2018</v>
       </c>
-      <c r="H18" t="s">
+      <c r="H18">
+        <v>2021</v>
+      </c>
+      <c r="I18" t="s">
         <v>14</v>
       </c>
-      <c r="I18" t="s">
+      <c r="J18" t="s">
         <v>3</v>
       </c>
-      <c r="J18" t="s">
+      <c r="K18" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>2</v>
       </c>
@@ -1338,7 +1622,7 @@
         <v>73</v>
       </c>
       <c r="C19" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>15</v>
@@ -1352,17 +1636,20 @@
       <c r="G19">
         <v>2005</v>
       </c>
-      <c r="H19" t="s">
+      <c r="H19">
+        <v>2021</v>
+      </c>
+      <c r="I19" t="s">
         <v>2</v>
       </c>
-      <c r="I19" t="s">
+      <c r="J19" t="s">
         <v>3</v>
       </c>
-      <c r="J19" t="s">
+      <c r="K19" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>2</v>
       </c>
@@ -1370,7 +1657,7 @@
         <v>67</v>
       </c>
       <c r="C20" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>34</v>
@@ -1384,17 +1671,20 @@
       <c r="G20">
         <v>2015</v>
       </c>
-      <c r="H20" t="s">
+      <c r="H20">
+        <v>2021</v>
+      </c>
+      <c r="I20" t="s">
         <v>17</v>
       </c>
-      <c r="I20" t="s">
+      <c r="J20" t="s">
         <v>10</v>
       </c>
-      <c r="J20" t="s">
+      <c r="K20" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>2</v>
       </c>
@@ -1402,7 +1692,7 @@
         <v>55</v>
       </c>
       <c r="C21" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>18</v>
@@ -1416,14 +1706,17 @@
       <c r="G21">
         <v>2015</v>
       </c>
-      <c r="H21" t="s">
+      <c r="H21">
+        <v>2021</v>
+      </c>
+      <c r="I21" t="s">
         <v>3</v>
       </c>
-      <c r="J21" t="s">
+      <c r="K21" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>3</v>
       </c>
@@ -1431,7 +1724,7 @@
         <v>62</v>
       </c>
       <c r="C22" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>21</v>
@@ -1445,14 +1738,17 @@
       <c r="G22">
         <v>2007</v>
       </c>
-      <c r="H22" t="s">
+      <c r="H22">
+        <v>2021</v>
+      </c>
+      <c r="I22" t="s">
         <v>22</v>
       </c>
-      <c r="J22" t="s">
+      <c r="K22" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>3</v>
       </c>
@@ -1460,7 +1756,7 @@
         <v>70</v>
       </c>
       <c r="C23" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>37</v>
@@ -1474,17 +1770,20 @@
       <c r="G23">
         <v>2015</v>
       </c>
-      <c r="H23" t="s">
+      <c r="H23">
+        <v>2021</v>
+      </c>
+      <c r="I23" t="s">
         <v>3</v>
       </c>
-      <c r="I23" t="s">
+      <c r="J23" t="s">
         <v>46</v>
       </c>
-      <c r="J23" t="s">
+      <c r="K23" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>3</v>
       </c>
@@ -1492,7 +1791,7 @@
         <v>78</v>
       </c>
       <c r="C24" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>20</v>
@@ -1506,17 +1805,20 @@
       <c r="G24">
         <v>2015</v>
       </c>
-      <c r="H24" t="s">
+      <c r="H24">
+        <v>2021</v>
+      </c>
+      <c r="I24" t="s">
         <v>3</v>
       </c>
-      <c r="I24" t="s">
+      <c r="J24" t="s">
         <v>46</v>
       </c>
-      <c r="J24" t="s">
+      <c r="K24" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>3</v>
       </c>
@@ -1524,7 +1826,7 @@
         <v>74</v>
       </c>
       <c r="C25" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>39</v>
@@ -1538,14 +1840,17 @@
       <c r="G25">
         <v>2019</v>
       </c>
-      <c r="H25" t="s">
+      <c r="H25">
+        <v>2021</v>
+      </c>
+      <c r="I25" t="s">
         <v>3</v>
       </c>
-      <c r="J25" t="s">
+      <c r="K25" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>3</v>
       </c>
@@ -1553,7 +1858,7 @@
         <v>75</v>
       </c>
       <c r="C26" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>40</v>
@@ -1567,17 +1872,20 @@
       <c r="G26">
         <v>2014</v>
       </c>
-      <c r="H26" t="s">
+      <c r="H26">
+        <v>2021</v>
+      </c>
+      <c r="I26" t="s">
         <v>3</v>
       </c>
-      <c r="I26" t="s">
+      <c r="J26" t="s">
         <v>2</v>
       </c>
-      <c r="J26" t="s">
+      <c r="K26" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>3</v>
       </c>
@@ -1585,7 +1893,7 @@
         <v>79</v>
       </c>
       <c r="C27" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>19</v>
@@ -1599,17 +1907,20 @@
       <c r="G27">
         <v>2016</v>
       </c>
-      <c r="H27" t="s">
+      <c r="H27">
+        <v>2021</v>
+      </c>
+      <c r="I27" t="s">
         <v>3</v>
       </c>
-      <c r="I27" t="s">
+      <c r="J27" t="s">
         <v>6</v>
       </c>
-      <c r="J27" t="s">
+      <c r="K27" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>3</v>
       </c>
@@ -1617,7 +1928,7 @@
         <v>71</v>
       </c>
       <c r="C28" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>38</v>
@@ -1631,17 +1942,20 @@
       <c r="G28">
         <v>2012</v>
       </c>
-      <c r="H28" t="s">
+      <c r="H28">
+        <v>2021</v>
+      </c>
+      <c r="I28" t="s">
         <v>2</v>
       </c>
-      <c r="I28" t="s">
+      <c r="J28" t="s">
         <v>6</v>
       </c>
-      <c r="J28" t="s">
+      <c r="K28" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>3</v>
       </c>
@@ -1649,7 +1963,7 @@
         <v>54</v>
       </c>
       <c r="C29" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>12</v>
@@ -1663,17 +1977,20 @@
       <c r="G29">
         <v>2018</v>
       </c>
-      <c r="H29" t="s">
+      <c r="H29">
+        <v>2021</v>
+      </c>
+      <c r="I29" t="s">
         <v>2</v>
       </c>
-      <c r="I29" t="s">
+      <c r="J29" t="s">
         <v>6</v>
       </c>
-      <c r="J29" t="s">
+      <c r="K29" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>3</v>
       </c>
@@ -1681,7 +1998,7 @@
         <v>63</v>
       </c>
       <c r="C30" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>30</v>
@@ -1695,14 +2012,17 @@
       <c r="G30">
         <v>2015</v>
       </c>
-      <c r="H30" t="s">
+      <c r="H30">
+        <v>2021</v>
+      </c>
+      <c r="I30" t="s">
         <v>3</v>
       </c>
-      <c r="J30" t="s">
+      <c r="K30" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>3</v>
       </c>
@@ -1710,7 +2030,7 @@
         <v>72</v>
       </c>
       <c r="C31" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>9</v>
@@ -1724,22 +2044,608 @@
       <c r="G31">
         <v>2014</v>
       </c>
-      <c r="H31" t="s">
+      <c r="H31">
+        <v>2021</v>
+      </c>
+      <c r="I31" t="s">
         <v>17</v>
       </c>
-      <c r="I31" t="s">
+      <c r="J31" t="s">
         <v>10</v>
       </c>
-      <c r="J31" t="s">
+      <c r="K31" t="s">
         <v>100</v>
       </c>
     </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>1</v>
+      </c>
+      <c r="B32" t="s">
+        <v>119</v>
+      </c>
+      <c r="C32" t="s">
+        <v>117</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="E32" t="s">
+        <v>147</v>
+      </c>
+      <c r="F32" t="s">
+        <v>154</v>
+      </c>
+      <c r="G32">
+        <v>2013</v>
+      </c>
+      <c r="H32">
+        <v>2021</v>
+      </c>
+      <c r="I32" t="s">
+        <v>164</v>
+      </c>
+      <c r="K32" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>1</v>
+      </c>
+      <c r="B33" t="s">
+        <v>120</v>
+      </c>
+      <c r="C33" t="s">
+        <v>117</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E33" t="s">
+        <v>148</v>
+      </c>
+      <c r="F33" t="s">
+        <v>154</v>
+      </c>
+      <c r="G33">
+        <v>2017</v>
+      </c>
+      <c r="H33">
+        <v>2021</v>
+      </c>
+      <c r="K33" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>1</v>
+      </c>
+      <c r="B34" t="s">
+        <v>121</v>
+      </c>
+      <c r="C34" t="s">
+        <v>117</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E34" t="s">
+        <v>148</v>
+      </c>
+      <c r="F34" t="s">
+        <v>154</v>
+      </c>
+      <c r="G34">
+        <v>2012</v>
+      </c>
+      <c r="H34">
+        <v>2021</v>
+      </c>
+      <c r="I34" t="s">
+        <v>3</v>
+      </c>
+      <c r="J34" t="s">
+        <v>14</v>
+      </c>
+      <c r="K34" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>1</v>
+      </c>
+      <c r="B35" t="s">
+        <v>122</v>
+      </c>
+      <c r="C35" t="s">
+        <v>117</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E35" t="s">
+        <v>149</v>
+      </c>
+      <c r="F35" t="s">
+        <v>154</v>
+      </c>
+      <c r="G35">
+        <v>2013</v>
+      </c>
+      <c r="H35">
+        <v>2021</v>
+      </c>
+      <c r="K35" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>1</v>
+      </c>
+      <c r="B36" t="s">
+        <v>123</v>
+      </c>
+      <c r="C36" t="s">
+        <v>117</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="E36" t="s">
+        <v>150</v>
+      </c>
+      <c r="F36" t="s">
+        <v>154</v>
+      </c>
+      <c r="G36">
+        <v>2013</v>
+      </c>
+      <c r="H36">
+        <v>2021</v>
+      </c>
+      <c r="K36" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>1</v>
+      </c>
+      <c r="B37" t="s">
+        <v>124</v>
+      </c>
+      <c r="C37" t="s">
+        <v>117</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="E37" t="s">
+        <v>148</v>
+      </c>
+      <c r="F37" t="s">
+        <v>154</v>
+      </c>
+      <c r="G37">
+        <v>2020</v>
+      </c>
+      <c r="H37">
+        <v>2021</v>
+      </c>
+      <c r="K37" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>1</v>
+      </c>
+      <c r="B38" t="s">
+        <v>125</v>
+      </c>
+      <c r="C38" t="s">
+        <v>117</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="E38" t="s">
+        <v>151</v>
+      </c>
+      <c r="F38" t="s">
+        <v>154</v>
+      </c>
+      <c r="H38">
+        <v>2021</v>
+      </c>
+      <c r="K38" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>1</v>
+      </c>
+      <c r="B39" t="s">
+        <v>126</v>
+      </c>
+      <c r="C39" t="s">
+        <v>117</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="E39" t="s">
+        <v>148</v>
+      </c>
+      <c r="F39" t="s">
+        <v>154</v>
+      </c>
+      <c r="G39">
+        <v>2014</v>
+      </c>
+      <c r="H39">
+        <v>2021</v>
+      </c>
+      <c r="K39" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>1</v>
+      </c>
+      <c r="B40" t="s">
+        <v>127</v>
+      </c>
+      <c r="C40" t="s">
+        <v>117</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="E40" t="s">
+        <v>152</v>
+      </c>
+      <c r="F40" t="s">
+        <v>154</v>
+      </c>
+      <c r="H40">
+        <v>2021</v>
+      </c>
+      <c r="K40" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>1</v>
+      </c>
+      <c r="B41" t="s">
+        <v>128</v>
+      </c>
+      <c r="C41" t="s">
+        <v>117</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E41" t="s">
+        <v>169</v>
+      </c>
+      <c r="F41" t="s">
+        <v>154</v>
+      </c>
+      <c r="G41">
+        <v>2009</v>
+      </c>
+      <c r="H41">
+        <v>2021</v>
+      </c>
+      <c r="K41" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>1</v>
+      </c>
+      <c r="B42" t="s">
+        <v>129</v>
+      </c>
+      <c r="C42" t="s">
+        <v>117</v>
+      </c>
+      <c r="D42" t="s">
+        <v>170</v>
+      </c>
+      <c r="E42" t="s">
+        <v>148</v>
+      </c>
+      <c r="F42" t="s">
+        <v>154</v>
+      </c>
+      <c r="G42">
+        <v>2017</v>
+      </c>
+      <c r="H42">
+        <v>2021</v>
+      </c>
+      <c r="K42" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>1</v>
+      </c>
+      <c r="B43" t="s">
+        <v>130</v>
+      </c>
+      <c r="C43" t="s">
+        <v>117</v>
+      </c>
+      <c r="D43" t="s">
+        <v>172</v>
+      </c>
+      <c r="E43" t="s">
+        <v>174</v>
+      </c>
+      <c r="F43" t="s">
+        <v>154</v>
+      </c>
+      <c r="G43">
+        <v>2014</v>
+      </c>
+      <c r="H43">
+        <v>2021</v>
+      </c>
+      <c r="K43" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>1</v>
+      </c>
+      <c r="B44" t="s">
+        <v>131</v>
+      </c>
+      <c r="C44" t="s">
+        <v>117</v>
+      </c>
+      <c r="D44" t="s">
+        <v>176</v>
+      </c>
+      <c r="E44" t="s">
+        <v>147</v>
+      </c>
+      <c r="F44" t="s">
+        <v>154</v>
+      </c>
+      <c r="G44">
+        <v>2017</v>
+      </c>
+      <c r="H44">
+        <v>2021</v>
+      </c>
+      <c r="K44" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>1</v>
+      </c>
+      <c r="B45" t="s">
+        <v>132</v>
+      </c>
+      <c r="C45" t="s">
+        <v>117</v>
+      </c>
+      <c r="D45" t="s">
+        <v>178</v>
+      </c>
+      <c r="E45" t="s">
+        <v>147</v>
+      </c>
+      <c r="F45" t="s">
+        <v>154</v>
+      </c>
+      <c r="G45">
+        <v>2018</v>
+      </c>
+      <c r="H45">
+        <v>2021</v>
+      </c>
+      <c r="K45" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>1</v>
+      </c>
+      <c r="B46" t="s">
+        <v>133</v>
+      </c>
+      <c r="C46" t="s">
+        <v>117</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E46" t="s">
+        <v>147</v>
+      </c>
+      <c r="F46" t="s">
+        <v>154</v>
+      </c>
+      <c r="G46">
+        <v>2014</v>
+      </c>
+      <c r="H46">
+        <v>2021</v>
+      </c>
+      <c r="K46" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>1</v>
+      </c>
+      <c r="B47" t="s">
+        <v>134</v>
+      </c>
+      <c r="C47" t="s">
+        <v>117</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E47" t="s">
+        <v>153</v>
+      </c>
+      <c r="F47" t="s">
+        <v>154</v>
+      </c>
+      <c r="G47">
+        <v>2007</v>
+      </c>
+      <c r="H47">
+        <v>2021</v>
+      </c>
+      <c r="K47" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>1</v>
+      </c>
+      <c r="B48" t="s">
+        <v>167</v>
+      </c>
+      <c r="C48" t="s">
+        <v>117</v>
+      </c>
+      <c r="D48" t="s">
+        <v>166</v>
+      </c>
+      <c r="E48" t="s">
+        <v>168</v>
+      </c>
+      <c r="F48" t="s">
+        <v>154</v>
+      </c>
+      <c r="G48">
+        <v>2015</v>
+      </c>
+      <c r="H48">
+        <v>2021</v>
+      </c>
+      <c r="K48" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>1</v>
+      </c>
+      <c r="B49" t="s">
+        <v>179</v>
+      </c>
+      <c r="C49" t="s">
+        <v>117</v>
+      </c>
+      <c r="D49" t="s">
+        <v>181</v>
+      </c>
+      <c r="E49" t="s">
+        <v>180</v>
+      </c>
+      <c r="F49" t="s">
+        <v>154</v>
+      </c>
+      <c r="G49">
+        <v>1981</v>
+      </c>
+      <c r="H49">
+        <v>2021</v>
+      </c>
+      <c r="K49" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>1</v>
+      </c>
+      <c r="B50" t="s">
+        <v>187</v>
+      </c>
+      <c r="C50" t="s">
+        <v>117</v>
+      </c>
+      <c r="D50" t="s">
+        <v>192</v>
+      </c>
+      <c r="E50" t="s">
+        <v>148</v>
+      </c>
+      <c r="F50" t="s">
+        <v>154</v>
+      </c>
+      <c r="G50">
+        <v>1998</v>
+      </c>
+      <c r="H50">
+        <v>2021</v>
+      </c>
+      <c r="K50" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>1</v>
+      </c>
+      <c r="B51" t="s">
+        <v>189</v>
+      </c>
+      <c r="C51" t="s">
+        <v>117</v>
+      </c>
+      <c r="D51" t="s">
+        <v>193</v>
+      </c>
+      <c r="E51" t="s">
+        <v>190</v>
+      </c>
+      <c r="F51" t="s">
+        <v>154</v>
+      </c>
+      <c r="G51">
+        <v>1994</v>
+      </c>
+      <c r="H51">
+        <v>2021</v>
+      </c>
+      <c r="K51" t="s">
+        <v>191</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J32">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K32">
     <sortCondition ref="A2:A32"/>
     <sortCondition ref="B2:B32"/>
   </sortState>
-  <conditionalFormatting sqref="D1:D14 E1:J1 D16:D1048576">
+  <conditionalFormatting sqref="D1:D14 F1:K1 D16:D1048576">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
@@ -1773,19 +2679,25 @@
     <hyperlink ref="D10" r:id="rId28" xr:uid="{C1303E58-40CE-41B3-A608-57923205F336}"/>
     <hyperlink ref="D14" r:id="rId29" xr:uid="{ABA4C35B-DE92-40E9-AE01-394A30574CDB}"/>
     <hyperlink ref="D15" r:id="rId30" xr:uid="{7FE26976-A1E4-4FA4-8979-73B1647C76BA}"/>
+    <hyperlink ref="D32" r:id="rId31" xr:uid="{CD4A7F1C-9CAE-3C43-A032-F00FD459F7A1}"/>
+    <hyperlink ref="D33" r:id="rId32" xr:uid="{27F0748C-C010-354D-8790-336B5F03234E}"/>
+    <hyperlink ref="D34" r:id="rId33" xr:uid="{7EC2B062-3457-DB45-A5CC-AAA6C6D747C0}"/>
+    <hyperlink ref="D35" r:id="rId34" xr:uid="{874B72F3-13DC-8241-9902-532EFC288234}"/>
+    <hyperlink ref="D36" r:id="rId35" xr:uid="{C470249C-7B6A-8D4B-8946-DAD4214D10A6}"/>
+    <hyperlink ref="D37" r:id="rId36" xr:uid="{E225CE6B-04B7-DF45-A0D9-6D65E393BB36}"/>
+    <hyperlink ref="D38" r:id="rId37" xr:uid="{326EAC19-65B7-7D43-BE18-F373B67C6E9F}"/>
+    <hyperlink ref="D39" r:id="rId38" xr:uid="{C522605C-014E-CE44-B4D8-DBE7CD10484E}"/>
+    <hyperlink ref="D40" r:id="rId39" xr:uid="{D01BD3F5-3A12-E745-AB03-3D1EE38515B9}"/>
+    <hyperlink ref="D41" r:id="rId40" xr:uid="{D41838A3-7358-B44E-8F54-2DF236EF4301}"/>
+    <hyperlink ref="D46" r:id="rId41" xr:uid="{FF33AE96-AE53-C146-8CCB-1AD7BCFABC66}"/>
+    <hyperlink ref="D47" r:id="rId42" xr:uid="{AF64A86E-0EC1-D24C-B1FA-5ED63CCFAF6E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId31"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId43"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -1794,7 +2706,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C4EEA5216B515E4DBEF97013190A83FF" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="082830f1cf2a2806fd1515ef5c5c6dd6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="5c8e5eb2-3a7f-4a58-bb00-90e9e7cf5698" xmlns:ns4="343c309e-8554-41d3-9842-95c1f19f66f5" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bad9b9f9705881cfa2b4e34bdb1dcdea" ns3:_="" ns4:_="">
     <xsd:import namespace="5c8e5eb2-3a7f-4a58-bb00-90e9e7cf5698"/>
@@ -2017,16 +2929,13 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0733DD8-2E83-4E79-9655-8E35F0C73914}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{948B56C4-BC62-41C6-94BB-8AC37748C146}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -2034,7 +2943,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F9517CA-BD9A-431D-9A71-A13F66F2241B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2051,4 +2960,13 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0733DD8-2E83-4E79-9655-8E35F0C73914}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>